<commit_message>
dataset adding to system
</commit_message>
<xml_diff>
--- a/Development Part/backup/dataset.xlsx
+++ b/Development Part/backup/dataset.xlsx
@@ -1422,9 +1422,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EA367"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A358" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C367" sqref="C367"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="133" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
All products added to system
</commit_message>
<xml_diff>
--- a/Development Part/backup/dataset.xlsx
+++ b/Development Part/backup/dataset.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="350">
   <si>
     <t>1F3GDEL</t>
   </si>
@@ -1066,6 +1066,9 @@
   </si>
   <si>
     <t>Wash</t>
+  </si>
+  <si>
+    <t>1B6</t>
   </si>
 </sst>
 </file>
@@ -1425,9 +1428,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EA367"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" zoomScale="133" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN1" sqref="AN1"/>
+      <selection pane="bottomLeft" activeCell="AS1" sqref="AS1:AS1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1652,7 +1655,7 @@
         <v>91</v>
       </c>
       <c r="AS1" t="s">
-        <v>44</v>
+        <v>349</v>
       </c>
       <c r="AT1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
All invoice generated using collected data
</commit_message>
<xml_diff>
--- a/Development Part/backup/dataset.xlsx
+++ b/Development Part/backup/dataset.xlsx
@@ -1429,8 +1429,8 @@
   <dimension ref="A1:EA367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AS1" sqref="AS1:AS1048576"/>
+      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B268" sqref="B268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8865,7 +8865,9 @@
       <c r="A268" s="4">
         <v>45078</v>
       </c>
-      <c r="B268" s="9"/>
+      <c r="B268" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="269" spans="1:104" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A269" s="4">

</xml_diff>